<commit_message>
fixed mm units and a few other small issues
</commit_message>
<xml_diff>
--- a/LTER_ForageFish_Info.xlsx
+++ b/LTER_ForageFish_Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfutrelle\Documents\GitHub\nes-lter-fish-diet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18486008-A8CF-455E-A29D-C99C8A3D7A87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED44FBA5-62BE-4B72-9C51-1441DFAA174D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13140" activeTab="1" xr2:uid="{20CBF2A6-5EEF-447F-A717-1AB3AC94F5B2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13140" xr2:uid="{20CBF2A6-5EEF-447F-A717-1AB3AC94F5B2}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="6" r:id="rId1"/>
@@ -455,9 +455,6 @@
     <t>Length of prey</t>
   </si>
   <si>
-    <t>millimeters</t>
-  </si>
-  <si>
     <t>microscope used for identification and measurments</t>
   </si>
   <si>
@@ -495,6 +492,9 @@
   </si>
   <si>
     <t>definition</t>
+  </si>
+  <si>
+    <t>millimeter</t>
   </si>
 </sst>
 </file>
@@ -892,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269705B7-DB6F-CA4E-AC53-B891847B83EE}">
   <dimension ref="A1:G16384"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -960,7 +960,7 @@
         <v>50</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -971,10 +971,7 @@
         <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -982,7 +979,7 @@
         <v>126</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>9</v>
@@ -994,7 +991,7 @@
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1022,7 +1019,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1039,7 +1036,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1055,8 +1052,11 @@
       <c r="D10" t="s">
         <v>10</v>
       </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
       <c r="G10" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1076,7 +1076,7 @@
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1090,13 +1090,13 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="F12" t="s">
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1104,10 +1104,10 @@
         <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1127,7 +1127,7 @@
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1149,7 +1149,7 @@
         <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>7</v>
@@ -1160,7 +1160,7 @@
         <v>113</v>
       </c>
       <c r="B17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>7</v>
@@ -1177,7 +1177,7 @@
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="F18" t="s">
         <v>2</v>
@@ -1198,7 +1198,7 @@
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>2</v>
@@ -1308,7 +1308,7 @@
         <v>136</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>2</v>
@@ -50393,7 +50393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1450A43-7CE0-8C4D-80E9-CDBE5E6D7720}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -50407,7 +50407,7 @@
         <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -50760,7 +50760,7 @@
         <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H4" t="s">
         <v>60</v>
@@ -50786,7 +50786,7 @@
         <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H5" t="s">
         <v>60</v>

</xml_diff>